<commit_message>
update 03 april 2023
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\new-inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\project-inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BBF445-49AE-4E11-B4E6-B2CE327AF385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0828874B-D57F-4E4B-95C6-0946FFCBCA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58EAB302-6F53-46DE-9F24-B5F63DB38A9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58EAB302-6F53-46DE-9F24-B5F63DB38A9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="167">
   <si>
     <t>Table Customer</t>
   </si>
@@ -1017,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5F7A83-68FB-4936-89E0-A2513F628D09}">
   <dimension ref="A1:I209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,14 +1936,10 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="A108" s="8"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
-        <v>36</v>
-      </c>
+      <c r="A109" s="8"/>
       <c r="G109" s="1" t="s">
         <v>129</v>
       </c>

</xml_diff>

<commit_message>
Update 14 April 2023
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\project-inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0828874B-D57F-4E4B-95C6-0946FFCBCA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A43718-C301-4DF1-B448-1CA0E32F07AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58EAB302-6F53-46DE-9F24-B5F63DB38A9B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="171">
   <si>
     <t>Table Customer</t>
   </si>
@@ -526,6 +526,18 @@
   </si>
   <si>
     <t>ongkos_kirim</t>
+  </si>
+  <si>
+    <t>id_ganti_merk_in</t>
+  </si>
+  <si>
+    <t>Table Peubahan Merk IN</t>
+  </si>
+  <si>
+    <t>Table Peubahan Merk Out</t>
+  </si>
+  <si>
+    <t>id_ganti_merk_out</t>
   </si>
 </sst>
 </file>
@@ -1015,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5F7A83-68FB-4936-89E0-A2513F628D09}">
-  <dimension ref="A1:I209"/>
+  <dimension ref="A1:I225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="G230" sqref="G230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2448,6 +2460,66 @@
         <v>70</v>
       </c>
     </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>